<commit_message>
Updated stencil timings for srlpi.
</commit_message>
<xml_diff>
--- a/results/srlpi-ARM.xlsx
+++ b/results/srlpi-ARM.xlsx
@@ -5,16 +5,16 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aktemur/Dropbox/Matrix/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aktemur/git/thundercat/results/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="26140" yWindow="7240" windowWidth="22660" windowHeight="17620" tabRatio="500"/>
+    <workbookView xWindow="6060" yWindow="440" windowWidth="22660" windowHeight="17560" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="GPCE matrices" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="150000" concurrentCalc="0"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -110,13 +110,13 @@
     <t>CSRbyNZ-a6d1617 speedup</t>
   </si>
   <si>
-    <t>stencil-1947ae</t>
-  </si>
-  <si>
-    <t>stencil-1947ae speedup</t>
-  </si>
-  <si>
     <t>NumStencils</t>
+  </si>
+  <si>
+    <t>stencil-4b82ec</t>
+  </si>
+  <si>
+    <t>stencil-4b82ec speedup</t>
   </si>
 </sst>
 </file>
@@ -459,7 +459,7 @@
   <dimension ref="A1:G24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -478,13 +478,13 @@
         <v>26</v>
       </c>
       <c r="E1" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="G1" s="2" t="s">
         <v>27</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
@@ -498,15 +498,15 @@
         <v>46191.9</v>
       </c>
       <c r="D2" s="1">
-        <f>B2/C2</f>
+        <f t="shared" ref="D2:D24" si="0">B2/C2</f>
         <v>0.9964192856323294</v>
       </c>
       <c r="E2">
-        <v>88439.6</v>
+        <v>71825.5</v>
       </c>
       <c r="F2" s="1">
-        <f>B2/E2</f>
-        <v>0.52042863151800778</v>
+        <f t="shared" ref="F2:F24" si="1">B2/E2</f>
+        <v>0.6408100187259399</v>
       </c>
       <c r="G2">
         <v>161683</v>
@@ -523,15 +523,15 @@
         <v>34159.300000000003</v>
       </c>
       <c r="D3" s="1">
-        <f>B3/C3</f>
+        <f t="shared" si="0"/>
         <v>0.80287066772445559</v>
       </c>
       <c r="E3">
-        <v>45898.8</v>
+        <v>41537</v>
       </c>
       <c r="F3" s="1">
-        <f>B3/E3</f>
-        <v>0.59752106808892602</v>
+        <f t="shared" si="1"/>
+        <v>0.66026675012639335</v>
       </c>
       <c r="G3">
         <v>31814</v>
@@ -548,15 +548,15 @@
         <v>41187.1</v>
       </c>
       <c r="D4" s="1">
-        <f>B4/C4</f>
+        <f t="shared" si="0"/>
         <v>0.84506799459053938</v>
       </c>
       <c r="E4">
-        <v>52270</v>
+        <v>48000.5</v>
       </c>
       <c r="F4" s="1">
-        <f>B4/E4</f>
-        <v>0.66588674191696962</v>
+        <f t="shared" si="1"/>
+        <v>0.72511536338163152</v>
       </c>
       <c r="G4">
         <v>49442</v>
@@ -573,15 +573,15 @@
         <v>44649.4</v>
       </c>
       <c r="D5" s="1">
-        <f>B5/C5</f>
+        <f t="shared" si="0"/>
         <v>0.9125251403154353</v>
       </c>
       <c r="E5">
-        <v>56528.5</v>
+        <v>51993.8</v>
       </c>
       <c r="F5" s="1">
-        <f>B5/E5</f>
-        <v>0.72076386247644986</v>
+        <f t="shared" si="1"/>
+        <v>0.78362612465332393</v>
       </c>
       <c r="G5">
         <v>40649</v>
@@ -598,15 +598,15 @@
         <v>98243</v>
       </c>
       <c r="D6" s="1">
-        <f>B6/C6</f>
+        <f t="shared" si="0"/>
         <v>0.89551621998513886</v>
       </c>
       <c r="E6">
-        <v>136781</v>
+        <v>119228</v>
       </c>
       <c r="F6" s="1">
-        <f>B6/E6</f>
-        <v>0.6432048310803401</v>
+        <f t="shared" si="1"/>
+        <v>0.7378988157144295</v>
       </c>
       <c r="G6">
         <v>126894</v>
@@ -623,15 +623,15 @@
         <v>241085</v>
       </c>
       <c r="D7" s="1">
-        <f>B7/C7</f>
+        <f t="shared" si="0"/>
         <v>0.89787419374909261</v>
       </c>
       <c r="E7">
-        <v>411277</v>
+        <v>343055</v>
       </c>
       <c r="F7" s="1">
-        <f>B7/E7</f>
-        <v>0.52632167614527436</v>
+        <f t="shared" si="1"/>
+        <v>0.63098919998251013</v>
       </c>
       <c r="G7">
         <v>504865</v>
@@ -648,15 +648,15 @@
         <v>24711</v>
       </c>
       <c r="D8" s="1">
-        <f>B8/C8</f>
+        <f t="shared" si="0"/>
         <v>0.89929586014325602</v>
       </c>
       <c r="E8">
-        <v>18265.5</v>
+        <v>18202.3</v>
       </c>
       <c r="F8" s="3">
-        <f>B8/E8</f>
-        <v>1.2166379239549971</v>
+        <f t="shared" si="1"/>
+        <v>1.2208621987331272</v>
       </c>
       <c r="G8">
         <v>601</v>
@@ -673,15 +673,15 @@
         <v>27295.3</v>
       </c>
       <c r="D9" s="1">
-        <f>B9/C9</f>
+        <f t="shared" si="0"/>
         <v>0.91588661784263237</v>
       </c>
       <c r="E9">
-        <v>20394.3</v>
+        <v>20364.3</v>
       </c>
       <c r="F9" s="3">
-        <f>B9/E9</f>
-        <v>1.2258032881736565</v>
+        <f t="shared" si="1"/>
+        <v>1.227609100239144</v>
       </c>
       <c r="G9">
         <v>4682</v>
@@ -698,15 +698,15 @@
         <v>32477.599999999999</v>
       </c>
       <c r="D10" s="1">
-        <f>B10/C10</f>
+        <f t="shared" si="0"/>
         <v>0.90736076557381096</v>
       </c>
       <c r="E10">
-        <v>40844.9</v>
+        <v>40897.699999999997</v>
       </c>
       <c r="F10" s="1">
-        <f>B10/E10</f>
-        <v>0.72148297584276133</v>
+        <f t="shared" si="1"/>
+        <v>0.72055152245725318</v>
       </c>
       <c r="G10">
         <v>8391</v>
@@ -723,15 +723,15 @@
         <v>56574.400000000001</v>
       </c>
       <c r="D11" s="1">
-        <f>B11/C11</f>
+        <f t="shared" si="0"/>
         <v>1.0524336095477813</v>
       </c>
       <c r="E11">
-        <v>119324</v>
+        <v>95015.8</v>
       </c>
       <c r="F11" s="1">
-        <f>B11/E11</f>
-        <v>0.49898427809996315</v>
+        <f t="shared" si="1"/>
+        <v>0.62664104285813516</v>
       </c>
       <c r="G11">
         <v>200200</v>
@@ -748,15 +748,15 @@
         <v>48898.3</v>
       </c>
       <c r="D12" s="1">
-        <f>B12/C12</f>
+        <f t="shared" si="0"/>
         <v>0.99702034631060787</v>
       </c>
       <c r="E12">
-        <v>30310</v>
+        <v>30332</v>
       </c>
       <c r="F12" s="3">
-        <f>B12/E12</f>
-        <v>1.6084658528538436</v>
+        <f t="shared" si="1"/>
+        <v>1.6072992219438216</v>
       </c>
       <c r="G12">
         <v>3148</v>
@@ -773,15 +773,15 @@
         <v>45886</v>
       </c>
       <c r="D13" s="1">
-        <f>B13/C13</f>
+        <f t="shared" si="0"/>
         <v>0.92067951009022364</v>
       </c>
       <c r="E13">
-        <v>39978.400000000001</v>
+        <v>39338.699999999997</v>
       </c>
       <c r="F13" s="3">
-        <f>B13/E13</f>
-        <v>1.0567281331919236</v>
+        <f t="shared" si="1"/>
+        <v>1.0739119493018328</v>
       </c>
       <c r="G13">
         <v>7432</v>
@@ -798,15 +798,15 @@
         <v>82337.899999999994</v>
       </c>
       <c r="D14" s="1">
-        <f>B14/C14</f>
+        <f t="shared" si="0"/>
         <v>0.86739642376111137</v>
       </c>
       <c r="E14">
-        <v>74524.7</v>
+        <v>71267.899999999994</v>
       </c>
       <c r="F14" s="1">
-        <f>B14/E14</f>
-        <v>0.95833461926046004</v>
+        <f t="shared" si="1"/>
+        <v>1.0021285880459507</v>
       </c>
       <c r="G14">
         <v>46535</v>
@@ -823,15 +823,15 @@
         <v>172417</v>
       </c>
       <c r="D15" s="1">
-        <f>B15/C15</f>
+        <f t="shared" si="0"/>
         <v>0.83438408045610357</v>
       </c>
       <c r="E15">
-        <v>220282</v>
+        <v>202234</v>
       </c>
       <c r="F15" s="1">
-        <f>B15/E15</f>
-        <v>0.6530810506532535</v>
+        <f t="shared" si="1"/>
+        <v>0.71136406341169145</v>
       </c>
       <c r="G15">
         <v>172130</v>
@@ -848,15 +848,15 @@
         <v>100535</v>
       </c>
       <c r="D16" s="1">
-        <f>B16/C16</f>
+        <f t="shared" si="0"/>
         <v>0.78791067787337754</v>
       </c>
       <c r="E16">
-        <v>74155.7</v>
+        <v>71218.399999999994</v>
       </c>
       <c r="F16" s="3">
-        <f>B16/E16</f>
-        <v>1.0681930047184507</v>
+        <f t="shared" si="1"/>
+        <v>1.1122490816979884</v>
       </c>
       <c r="G16">
         <v>935</v>
@@ -873,15 +873,15 @@
         <v>80730.3</v>
       </c>
       <c r="D17" s="1">
-        <f>B17/C17</f>
+        <f t="shared" si="0"/>
         <v>0.98087582976899612</v>
       </c>
       <c r="E17">
-        <v>80104.399999999994</v>
+        <v>79437.5</v>
       </c>
       <c r="F17" s="1">
-        <f>B17/E17</f>
-        <v>0.98853995535825745</v>
+        <f t="shared" si="1"/>
+        <v>0.99683902439024386</v>
       </c>
       <c r="G17">
         <v>648</v>
@@ -898,15 +898,15 @@
         <v>139688</v>
       </c>
       <c r="D18" s="1">
-        <f>B18/C18</f>
+        <f t="shared" si="0"/>
         <v>0.60674360002290817</v>
       </c>
       <c r="E18">
-        <v>135333</v>
+        <v>127481</v>
       </c>
       <c r="F18" s="1">
-        <f>B18/E18</f>
-        <v>0.62626853760723555</v>
+        <f t="shared" si="1"/>
+        <v>0.66484260399588957</v>
       </c>
       <c r="G18">
         <v>105098</v>
@@ -923,15 +923,15 @@
         <v>114087</v>
       </c>
       <c r="D19" s="1">
-        <f>B19/C19</f>
+        <f t="shared" si="0"/>
         <v>0.88269478555838965</v>
       </c>
       <c r="E19">
-        <v>177607</v>
+        <v>163021</v>
       </c>
       <c r="F19" s="1">
-        <f>B19/E19</f>
-        <v>0.56700467886963912</v>
+        <f t="shared" si="1"/>
+        <v>0.61773636525355624</v>
       </c>
       <c r="G19">
         <v>130228</v>
@@ -948,15 +948,15 @@
         <v>166339</v>
       </c>
       <c r="D20" s="1">
-        <f>B20/C20</f>
+        <f t="shared" si="0"/>
         <v>1.0257726690673865</v>
       </c>
       <c r="E20">
-        <v>411609</v>
+        <v>295181</v>
       </c>
       <c r="F20" s="1">
-        <f>B20/E20</f>
-        <v>0.41453418171128426</v>
+        <f t="shared" si="1"/>
+        <v>0.57803855939237281</v>
       </c>
       <c r="G20">
         <v>786432</v>
@@ -973,15 +973,15 @@
         <v>116743</v>
       </c>
       <c r="D21" s="1">
-        <f>B21/C21</f>
+        <f t="shared" si="0"/>
         <v>1.0544529436454435</v>
       </c>
       <c r="E21">
-        <v>90685.5</v>
+        <v>91989.4</v>
       </c>
       <c r="F21" s="3">
-        <f>B21/E21</f>
-        <v>1.3574386202865949</v>
+        <f t="shared" si="1"/>
+        <v>1.3381976619045239</v>
       </c>
       <c r="G21">
         <v>2298</v>
@@ -998,15 +998,15 @@
         <v>117564</v>
       </c>
       <c r="D22" s="1">
-        <f>B22/C22</f>
+        <f t="shared" si="0"/>
         <v>0.79444472797795251</v>
       </c>
       <c r="E22">
-        <v>88099.6</v>
+        <v>88541.2</v>
       </c>
       <c r="F22" s="3">
-        <f>B22/E22</f>
-        <v>1.0601421572856176</v>
+        <f t="shared" si="1"/>
+        <v>1.0548546891164792</v>
       </c>
       <c r="G22">
         <v>1131</v>
@@ -1023,15 +1023,15 @@
         <v>168671</v>
       </c>
       <c r="D23" s="1">
-        <f>B23/C23</f>
+        <f t="shared" si="0"/>
         <v>0.68940718914336196</v>
       </c>
       <c r="E23">
-        <v>164928</v>
+        <v>157507</v>
       </c>
       <c r="F23" s="1">
-        <f>B23/E23</f>
-        <v>0.70505311408614668</v>
+        <f t="shared" si="1"/>
+        <v>0.73827194981810329</v>
       </c>
       <c r="G23">
         <v>84195</v>
@@ -1048,15 +1048,15 @@
         <v>203340</v>
       </c>
       <c r="D24" s="1">
-        <f>B24/C24</f>
+        <f t="shared" si="0"/>
         <v>0.96756171928789225</v>
       </c>
       <c r="E24">
-        <v>315913</v>
+        <v>293535</v>
       </c>
       <c r="F24" s="1">
-        <f>B24/E24</f>
-        <v>0.62277905625915997</v>
+        <f t="shared" si="1"/>
+        <v>0.6702573798695215</v>
       </c>
       <c r="G24">
         <v>204290</v>

</xml_diff>

<commit_message>
srlpi results for CSRbyNZ when using LDM and VLDM. No improvement observed.
</commit_message>
<xml_diff>
--- a/results/srlpi-ARM.xlsx
+++ b/results/srlpi-ARM.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="6060" yWindow="440" windowWidth="22660" windowHeight="17560" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="25220" yWindow="6520" windowWidth="22660" windowHeight="17560" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="GPCE matrices" sheetId="1" r:id="rId1"/>
@@ -333,10 +333,10 @@
     <t>NumRowLengths</t>
   </si>
   <si>
-    <t>CSRbyNZ-1e81f3</t>
-  </si>
-  <si>
     <t>stencil-1e81f3</t>
+  </si>
+  <si>
+    <t>CSRbyNZ-71f0de</t>
   </si>
 </sst>
 </file>
@@ -723,7 +723,7 @@
         <v>24</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>96</v>
@@ -732,7 +732,7 @@
         <v>100</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="I1" s="2" t="s">
         <v>97</v>
@@ -755,11 +755,11 @@
         <v>46026.5</v>
       </c>
       <c r="E2">
-        <v>45765</v>
+        <v>45762.2</v>
       </c>
       <c r="F2" s="1">
         <f t="shared" ref="F2:F24" si="0">D2/E2</f>
-        <v>1.0057139735605811</v>
+        <v>1.0057755090445828</v>
       </c>
       <c r="G2">
         <v>311</v>
@@ -789,11 +789,11 @@
         <v>27425.5</v>
       </c>
       <c r="E3">
-        <v>33181.800000000003</v>
+        <v>32806.400000000001</v>
       </c>
       <c r="F3" s="1">
         <f t="shared" si="0"/>
-        <v>0.82652237069718937</v>
+        <v>0.83598017460007801</v>
       </c>
       <c r="G3">
         <v>162</v>
@@ -823,11 +823,11 @@
         <v>34805.9</v>
       </c>
       <c r="E4">
-        <v>39829.199999999997</v>
+        <v>39503.1</v>
       </c>
       <c r="F4" s="1">
         <f t="shared" si="0"/>
-        <v>0.87387896317274771</v>
+        <v>0.88109287625528132</v>
       </c>
       <c r="G4">
         <v>326</v>
@@ -857,11 +857,11 @@
         <v>40743.699999999997</v>
       </c>
       <c r="E5">
-        <v>43773.7</v>
+        <v>43674.2</v>
       </c>
       <c r="F5" s="1">
         <f t="shared" si="0"/>
-        <v>0.93078035441372331</v>
+        <v>0.93290088885428923</v>
       </c>
       <c r="G5">
         <v>279</v>
@@ -891,11 +891,11 @@
         <v>87978.2</v>
       </c>
       <c r="E6">
-        <v>94690</v>
+        <v>93737.4</v>
       </c>
       <c r="F6" s="1">
         <f t="shared" si="0"/>
-        <v>0.92911817509768713</v>
+        <v>0.93856027583440549</v>
       </c>
       <c r="G6">
         <v>312</v>
@@ -925,11 +925,11 @@
         <v>216464</v>
       </c>
       <c r="E7">
-        <v>237733</v>
+        <v>234662</v>
       </c>
       <c r="F7" s="1">
         <f t="shared" si="0"/>
-        <v>0.91053408655929136</v>
+        <v>0.92245016236118327</v>
       </c>
       <c r="G7">
         <v>370</v>
@@ -959,11 +959,11 @@
         <v>22222.5</v>
       </c>
       <c r="E8">
-        <v>23887.7</v>
+        <v>23595.4</v>
       </c>
       <c r="F8" s="1">
         <f t="shared" si="0"/>
-        <v>0.93029048422409855</v>
+        <v>0.9418149300287344</v>
       </c>
       <c r="G8">
         <v>25</v>
@@ -993,11 +993,11 @@
         <v>24999.4</v>
       </c>
       <c r="E9">
-        <v>26438.2</v>
+        <v>26264.400000000001</v>
       </c>
       <c r="F9" s="1">
         <f t="shared" si="0"/>
-        <v>0.9455787459055458</v>
+        <v>0.95183594523385262</v>
       </c>
       <c r="G9">
         <v>22</v>
@@ -1027,11 +1027,11 @@
         <v>29468.9</v>
       </c>
       <c r="E10">
-        <v>31065.7</v>
+        <v>30892.6</v>
       </c>
       <c r="F10" s="1">
         <f t="shared" si="0"/>
-        <v>0.94859925898981834</v>
+        <v>0.95391452969319523</v>
       </c>
       <c r="G10">
         <v>70</v>
@@ -1061,11 +1061,11 @@
         <v>59540.800000000003</v>
       </c>
       <c r="E11">
-        <v>56600.4</v>
+        <v>56036.9</v>
       </c>
       <c r="F11" s="1">
         <f t="shared" si="0"/>
-        <v>1.0519501628963752</v>
+        <v>1.0625284410807878</v>
       </c>
       <c r="G11">
         <v>1</v>
@@ -1095,11 +1095,11 @@
         <v>48752.6</v>
       </c>
       <c r="E12">
-        <v>47079.5</v>
+        <v>46687.4</v>
       </c>
       <c r="F12" s="1">
         <f t="shared" si="0"/>
-        <v>1.035537760596438</v>
+        <v>1.0442346328988121</v>
       </c>
       <c r="G12">
         <v>3</v>
@@ -1129,11 +1129,11 @@
         <v>42246.3</v>
       </c>
       <c r="E13">
-        <v>44227</v>
+        <v>44015.3</v>
       </c>
       <c r="F13" s="1">
         <f t="shared" si="0"/>
-        <v>0.95521514007280628</v>
+        <v>0.95980942990278384</v>
       </c>
       <c r="G13">
         <v>71</v>
@@ -1163,11 +1163,11 @@
         <v>71419.600000000006</v>
       </c>
       <c r="E14">
-        <v>79455</v>
+        <v>80062.5</v>
       </c>
       <c r="F14" s="1">
         <f t="shared" si="0"/>
-        <v>0.89886854194197985</v>
+        <v>0.89204808743169406</v>
       </c>
       <c r="G14">
         <v>27</v>
@@ -1197,11 +1197,11 @@
         <v>143862</v>
       </c>
       <c r="E15">
-        <v>170867</v>
+        <v>171609</v>
       </c>
       <c r="F15" s="1">
         <f t="shared" si="0"/>
-        <v>0.84195309802360896</v>
+        <v>0.83831267590860614</v>
       </c>
       <c r="G15">
         <v>22</v>
@@ -1231,11 +1231,11 @@
         <v>79212.600000000006</v>
       </c>
       <c r="E16">
-        <v>96361.9</v>
+        <v>97190.1</v>
       </c>
       <c r="F16" s="1">
         <f t="shared" si="0"/>
-        <v>0.82203235926232265</v>
+        <v>0.81502745650019914</v>
       </c>
       <c r="G16">
         <v>23</v>
@@ -1265,11 +1265,11 @@
         <v>79186.399999999994</v>
       </c>
       <c r="E17">
-        <v>76081.399999999994</v>
+        <v>76615.7</v>
       </c>
       <c r="F17" s="1">
         <f t="shared" si="0"/>
-        <v>1.0408115518379</v>
+        <v>1.033553175132512</v>
       </c>
       <c r="G17">
         <v>1</v>
@@ -1299,11 +1299,11 @@
         <v>84754.8</v>
       </c>
       <c r="E18">
-        <v>136923</v>
+        <v>136559</v>
       </c>
       <c r="F18" s="1">
         <f t="shared" si="0"/>
-        <v>0.61899607808768431</v>
+        <v>0.62064602113372247</v>
       </c>
       <c r="G18">
         <v>60</v>
@@ -1333,11 +1333,11 @@
         <v>100704</v>
       </c>
       <c r="E19">
-        <v>111023</v>
+        <v>110779</v>
       </c>
       <c r="F19" s="1">
         <f t="shared" si="0"/>
-        <v>0.90705529484881509</v>
+        <v>0.90905315989492597</v>
       </c>
       <c r="G19">
         <v>28</v>
@@ -1367,11 +1367,11 @@
         <v>170626</v>
       </c>
       <c r="E20">
-        <v>163806</v>
+        <v>162576</v>
       </c>
       <c r="F20" s="1">
         <f t="shared" si="0"/>
-        <v>1.0416346165586121</v>
+        <v>1.0495153036118492</v>
       </c>
       <c r="G20">
         <v>3</v>
@@ -1401,11 +1401,11 @@
         <v>123100</v>
       </c>
       <c r="E21">
-        <v>116582</v>
+        <v>116919</v>
       </c>
       <c r="F21" s="1">
         <f t="shared" si="0"/>
-        <v>1.0559091454941587</v>
+        <v>1.0528656591315355</v>
       </c>
       <c r="G21">
         <v>3</v>
@@ -1435,11 +1435,11 @@
         <v>93398.1</v>
       </c>
       <c r="E22">
-        <v>111744</v>
+        <v>111296</v>
       </c>
       <c r="F22" s="1">
         <f t="shared" si="0"/>
-        <v>0.8358220575601375</v>
+        <v>0.83918649367452569</v>
       </c>
       <c r="G22">
         <v>29</v>
@@ -1469,11 +1469,11 @@
         <v>116283</v>
       </c>
       <c r="E23">
-        <v>166204</v>
+        <v>165427</v>
       </c>
       <c r="F23" s="1">
         <f t="shared" si="0"/>
-        <v>0.6996402011985271</v>
+        <v>0.70292636631263339</v>
       </c>
       <c r="G23">
         <v>147</v>
@@ -1503,11 +1503,11 @@
         <v>196744</v>
       </c>
       <c r="E24">
-        <v>201405</v>
+        <v>198853</v>
       </c>
       <c r="F24" s="1">
         <f t="shared" si="0"/>
-        <v>0.97685757553188846</v>
+        <v>0.98939417559704912</v>
       </c>
       <c r="G24">
         <v>9</v>
@@ -1533,7 +1533,7 @@
   <dimension ref="A1:J71"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L1" sqref="L1"/>
+      <selection activeCell="L2" sqref="L2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1556,7 +1556,7 @@
         <v>24</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>96</v>
@@ -1565,7 +1565,7 @@
         <v>100</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="I1" s="2" t="s">
         <v>97</v>
@@ -1588,11 +1588,11 @@
         <v>262.42099999999999</v>
       </c>
       <c r="E2">
-        <v>235.709</v>
+        <v>231.46</v>
       </c>
       <c r="F2" s="1">
         <f>D2/E2</f>
-        <v>1.1133261776173162</v>
+        <v>1.1337639332930096</v>
       </c>
       <c r="G2">
         <v>48</v>
@@ -1622,11 +1622,11 @@
         <v>446.416</v>
       </c>
       <c r="E3">
-        <v>404.44900000000001</v>
+        <v>423.01900000000001</v>
       </c>
       <c r="F3" s="1">
         <f t="shared" ref="F3:F66" si="0">D3/E3</f>
-        <v>1.1037633916760827</v>
+        <v>1.0553095723832735</v>
       </c>
       <c r="G3">
         <v>6</v>
@@ -1656,11 +1656,11 @@
         <v>272.60500000000002</v>
       </c>
       <c r="E4">
-        <v>244.167</v>
+        <v>244.57</v>
       </c>
       <c r="F4" s="1">
         <f t="shared" si="0"/>
-        <v>1.1164694655706955</v>
+        <v>1.1146297583513924</v>
       </c>
       <c r="G4">
         <v>31</v>
@@ -1690,11 +1690,11 @@
         <v>484.63200000000001</v>
       </c>
       <c r="E5">
-        <v>380.06700000000001</v>
+        <v>366.11599999999999</v>
       </c>
       <c r="F5" s="1">
         <f t="shared" si="0"/>
-        <v>1.2751225441829992</v>
+        <v>1.3237116105278108</v>
       </c>
       <c r="G5">
         <v>35</v>
@@ -1724,11 +1724,11 @@
         <v>260.88200000000001</v>
       </c>
       <c r="E6">
-        <v>228.107</v>
+        <v>223.59899999999999</v>
       </c>
       <c r="F6" s="1">
         <f t="shared" si="0"/>
-        <v>1.1436825700219635</v>
+        <v>1.1667404594832715</v>
       </c>
       <c r="G6">
         <v>17</v>
@@ -1758,11 +1758,11 @@
         <v>95.5535</v>
       </c>
       <c r="E7">
-        <v>76.119900000000001</v>
+        <v>75.023499999999999</v>
       </c>
       <c r="F7" s="1">
         <f t="shared" si="0"/>
-        <v>1.2553024898876641</v>
+        <v>1.273647590421668</v>
       </c>
       <c r="G7">
         <v>10</v>
@@ -1792,11 +1792,11 @@
         <v>108.357</v>
       </c>
       <c r="E8">
-        <v>86.8232</v>
+        <v>85.415000000000006</v>
       </c>
       <c r="F8" s="1">
         <f t="shared" si="0"/>
-        <v>1.2480189626735712</v>
+        <v>1.2685945091611543</v>
       </c>
       <c r="G8">
         <v>10</v>
@@ -1826,11 +1826,11 @@
         <v>68.049599999999998</v>
       </c>
       <c r="E9">
-        <v>58.013199999999998</v>
+        <v>57.622100000000003</v>
       </c>
       <c r="F9" s="1">
         <f t="shared" si="0"/>
-        <v>1.1730020064399136</v>
+        <v>1.1809635539142098</v>
       </c>
       <c r="G9">
         <v>17</v>
@@ -1860,11 +1860,11 @@
         <v>505.75200000000001</v>
       </c>
       <c r="E10">
-        <v>595.93600000000004</v>
+        <v>520.11599999999999</v>
       </c>
       <c r="F10" s="1">
         <f t="shared" si="0"/>
-        <v>0.84866831337593296</v>
+        <v>0.97238308377361982</v>
       </c>
       <c r="G10">
         <v>35</v>
@@ -1894,11 +1894,11 @@
         <v>76.725899999999996</v>
       </c>
       <c r="E11">
-        <v>64.263800000000003</v>
+        <v>63.741799999999998</v>
       </c>
       <c r="F11" s="1">
         <f t="shared" si="0"/>
-        <v>1.1939209944012024</v>
+        <v>1.2036983580633116</v>
       </c>
       <c r="G11">
         <v>9</v>
@@ -1928,11 +1928,11 @@
         <v>287.47899999999998</v>
       </c>
       <c r="E12">
-        <v>264.57900000000001</v>
+        <v>260.68200000000002</v>
       </c>
       <c r="F12" s="1">
         <f t="shared" si="0"/>
-        <v>1.0865525986567339</v>
+        <v>1.1027957434728901</v>
       </c>
       <c r="G12">
         <v>26</v>
@@ -1962,11 +1962,11 @@
         <v>59.801400000000001</v>
       </c>
       <c r="E13">
-        <v>51.197899999999997</v>
+        <v>51.012799999999999</v>
       </c>
       <c r="F13" s="1">
         <f t="shared" si="0"/>
-        <v>1.1680440018047615</v>
+        <v>1.1722822507292288</v>
       </c>
       <c r="G13">
         <v>12</v>
@@ -1996,11 +1996,11 @@
         <v>182.61</v>
       </c>
       <c r="E14">
-        <v>155.54400000000001</v>
+        <v>154.691</v>
       </c>
       <c r="F14" s="1">
         <f t="shared" si="0"/>
-        <v>1.1740086406418762</v>
+        <v>1.1804823810047127</v>
       </c>
       <c r="G14">
         <v>12</v>
@@ -2030,11 +2030,11 @@
         <v>93.410300000000007</v>
       </c>
       <c r="E15">
-        <v>78.713999999999999</v>
+        <v>78.396600000000007</v>
       </c>
       <c r="F15" s="1">
         <f t="shared" si="0"/>
-        <v>1.1867050334120997</v>
+        <v>1.1915095807726355</v>
       </c>
       <c r="G15">
         <v>30</v>
@@ -2064,11 +2064,11 @@
         <v>187.89699999999999</v>
       </c>
       <c r="E16">
-        <v>158.63800000000001</v>
+        <v>158.05199999999999</v>
       </c>
       <c r="F16" s="1">
         <f t="shared" si="0"/>
-        <v>1.1844387851586631</v>
+        <v>1.1888302583959709</v>
       </c>
       <c r="G16">
         <v>30</v>
@@ -2098,11 +2098,11 @@
         <v>426.18299999999999</v>
       </c>
       <c r="E17">
-        <v>355.18799999999999</v>
+        <v>360.495</v>
       </c>
       <c r="F17" s="1">
         <f t="shared" si="0"/>
-        <v>1.1998800635156592</v>
+        <v>1.1822161195023508</v>
       </c>
       <c r="G17">
         <v>48</v>
@@ -2132,11 +2132,11 @@
         <v>127.92700000000001</v>
       </c>
       <c r="E18">
-        <v>110.998</v>
+        <v>110.435</v>
       </c>
       <c r="F18" s="1">
         <f t="shared" si="0"/>
-        <v>1.1525162615542623</v>
+        <v>1.1583918141893421</v>
       </c>
       <c r="G18">
         <v>13</v>
@@ -2166,11 +2166,11 @@
         <v>71.954800000000006</v>
       </c>
       <c r="E19">
-        <v>60.886200000000002</v>
+        <v>60.49</v>
       </c>
       <c r="F19" s="1">
         <f t="shared" si="0"/>
-        <v>1.1817916046657535</v>
+        <v>1.1895321540750539</v>
       </c>
       <c r="G19">
         <v>20</v>
@@ -2200,11 +2200,11 @@
         <v>487.334</v>
       </c>
       <c r="E20">
-        <v>496.32499999999999</v>
+        <v>521.30999999999995</v>
       </c>
       <c r="F20" s="1">
         <f t="shared" si="0"/>
-        <v>0.98188485367450762</v>
+        <v>0.93482572749419746</v>
       </c>
       <c r="G20">
         <v>30</v>
@@ -2234,11 +2234,11 @@
         <v>90.608199999999997</v>
       </c>
       <c r="E21">
-        <v>78.007400000000004</v>
+        <v>76.860299999999995</v>
       </c>
       <c r="F21" s="1">
         <f t="shared" si="0"/>
-        <v>1.1615333929857936</v>
+        <v>1.1788686747254435</v>
       </c>
       <c r="G21">
         <v>3</v>
@@ -2268,11 +2268,11 @@
         <v>70.848699999999994</v>
       </c>
       <c r="E22">
-        <v>60.493099999999998</v>
+        <v>59.482500000000002</v>
       </c>
       <c r="F22" s="1">
         <f t="shared" si="0"/>
-        <v>1.1711864658944573</v>
+        <v>1.1910847728323455</v>
       </c>
       <c r="G22">
         <v>8</v>
@@ -2302,11 +2302,11 @@
         <v>310.84100000000001</v>
       </c>
       <c r="E23">
-        <v>288.548</v>
+        <v>287.75799999999998</v>
       </c>
       <c r="F23" s="1">
         <f t="shared" si="0"/>
-        <v>1.0772592428296159</v>
+        <v>1.0802167098742694</v>
       </c>
       <c r="G23">
         <v>39</v>
@@ -2336,11 +2336,11 @@
         <v>1978.06</v>
       </c>
       <c r="E24">
-        <v>1863.94</v>
+        <v>1844.26</v>
       </c>
       <c r="F24" s="1">
         <f t="shared" si="0"/>
-        <v>1.0612251467321909</v>
+        <v>1.0725494236170605</v>
       </c>
       <c r="G24">
         <v>3</v>
@@ -2370,11 +2370,11 @@
         <v>200.803</v>
       </c>
       <c r="E25">
-        <v>174.506</v>
+        <v>171.297</v>
       </c>
       <c r="F25" s="1">
         <f t="shared" si="0"/>
-        <v>1.1506939589469702</v>
+        <v>1.1722505356194213</v>
       </c>
       <c r="G25">
         <v>5</v>
@@ -2404,11 +2404,11 @@
         <v>117.55500000000001</v>
       </c>
       <c r="E26">
-        <v>100.812</v>
+        <v>99.603499999999997</v>
       </c>
       <c r="F26" s="1">
         <f t="shared" si="0"/>
-        <v>1.166081418878705</v>
+        <v>1.180229610405257</v>
       </c>
       <c r="G26">
         <v>9</v>
@@ -2438,11 +2438,11 @@
         <v>278.48700000000002</v>
       </c>
       <c r="E27">
-        <v>249.69800000000001</v>
+        <v>248.893</v>
       </c>
       <c r="F27" s="1">
         <f t="shared" si="0"/>
-        <v>1.1152952766942468</v>
+        <v>1.118902500271201</v>
       </c>
       <c r="G27">
         <v>14</v>
@@ -2472,11 +2472,11 @@
         <v>37.204599999999999</v>
       </c>
       <c r="E28">
-        <v>28.7759</v>
+        <v>28.1036</v>
       </c>
       <c r="F28" s="1">
         <f t="shared" si="0"/>
-        <v>1.2929083017386076</v>
+        <v>1.3238375154784441</v>
       </c>
       <c r="G28">
         <v>12</v>
@@ -2506,11 +2506,11 @@
         <v>83.347700000000003</v>
       </c>
       <c r="E29">
-        <v>75.012799999999999</v>
+        <v>75.463200000000001</v>
       </c>
       <c r="F29" s="1">
         <f t="shared" si="0"/>
-        <v>1.1111130367084019</v>
+        <v>1.1044813896044694</v>
       </c>
       <c r="G29">
         <v>19</v>
@@ -2540,11 +2540,11 @@
         <v>113.194</v>
       </c>
       <c r="E30">
-        <v>94.689099999999996</v>
+        <v>94.818200000000004</v>
       </c>
       <c r="F30" s="1">
         <f t="shared" si="0"/>
-        <v>1.1954279848472529</v>
+        <v>1.1938003463470093</v>
       </c>
       <c r="G30">
         <v>25</v>
@@ -2574,11 +2574,11 @@
         <v>320.86</v>
       </c>
       <c r="E31">
-        <v>141.315</v>
+        <v>141.95500000000001</v>
       </c>
       <c r="F31" s="1">
         <f t="shared" si="0"/>
-        <v>2.2705303754024699</v>
+        <v>2.2602937550632243</v>
       </c>
       <c r="G31">
         <v>57</v>
@@ -2608,11 +2608,11 @@
         <v>379.47800000000001</v>
       </c>
       <c r="E32">
-        <v>369.911</v>
+        <v>359.22800000000001</v>
       </c>
       <c r="F32" s="1">
         <f t="shared" si="0"/>
-        <v>1.0258629778514292</v>
+        <v>1.0563708842295143</v>
       </c>
       <c r="G32">
         <v>22</v>
@@ -2642,11 +2642,11 @@
         <v>119.764</v>
       </c>
       <c r="E33">
-        <v>102.613</v>
+        <v>101.134</v>
       </c>
       <c r="F33" s="1">
         <f t="shared" si="0"/>
-        <v>1.16714256478224</v>
+        <v>1.1842110467300808</v>
       </c>
       <c r="G33">
         <v>8</v>
@@ -2676,11 +2676,11 @@
         <v>100.608</v>
       </c>
       <c r="E34">
-        <v>87.296999999999997</v>
+        <v>87.821600000000004</v>
       </c>
       <c r="F34" s="1">
         <f t="shared" si="0"/>
-        <v>1.1524794666483384</v>
+        <v>1.1455951610993196</v>
       </c>
       <c r="G34">
         <v>19</v>
@@ -2710,11 +2710,11 @@
         <v>116.212</v>
       </c>
       <c r="E35">
-        <v>92.045900000000003</v>
+        <v>92.072500000000005</v>
       </c>
       <c r="F35" s="1">
         <f t="shared" si="0"/>
-        <v>1.2625440133672439</v>
+        <v>1.2621792609085232</v>
       </c>
       <c r="G35">
         <v>4</v>
@@ -2744,11 +2744,11 @@
         <v>164.00800000000001</v>
       </c>
       <c r="E36">
-        <v>140.678</v>
+        <v>139.36600000000001</v>
       </c>
       <c r="F36" s="1">
         <f t="shared" si="0"/>
-        <v>1.1658397190747667</v>
+        <v>1.1768150050944994</v>
       </c>
       <c r="G36">
         <v>39</v>
@@ -2778,11 +2778,11 @@
         <v>84.011399999999995</v>
       </c>
       <c r="E37">
-        <v>71.458399999999997</v>
+        <v>69.9405</v>
       </c>
       <c r="F37" s="1">
         <f t="shared" si="0"/>
-        <v>1.1756686407756121</v>
+        <v>1.2011838634267697</v>
       </c>
       <c r="G37">
         <v>5</v>
@@ -2812,11 +2812,11 @@
         <v>112.96599999999999</v>
       </c>
       <c r="E38">
-        <v>97.056600000000003</v>
+        <v>95.511399999999995</v>
       </c>
       <c r="F38" s="1">
         <f t="shared" si="0"/>
-        <v>1.1639187855333897</v>
+        <v>1.1827488655804439</v>
       </c>
       <c r="G38">
         <v>6</v>
@@ -2846,11 +2846,11 @@
         <v>68.322299999999998</v>
       </c>
       <c r="E39">
-        <v>59.298400000000001</v>
+        <v>58.9955</v>
       </c>
       <c r="F39" s="1">
         <f t="shared" si="0"/>
-        <v>1.1521777990637183</v>
+        <v>1.1580934139044503</v>
       </c>
       <c r="G39">
         <v>24</v>
@@ -2880,11 +2880,11 @@
         <v>115.136</v>
       </c>
       <c r="E40">
-        <v>98.962800000000001</v>
+        <v>97.951800000000006</v>
       </c>
       <c r="F40" s="1">
         <f t="shared" si="0"/>
-        <v>1.1634270655236107</v>
+        <v>1.1754352650997735</v>
       </c>
       <c r="G40">
         <v>13</v>
@@ -2914,11 +2914,11 @@
         <v>487.03399999999999</v>
       </c>
       <c r="E41">
-        <v>449.83800000000002</v>
+        <v>454.71199999999999</v>
       </c>
       <c r="F41" s="1">
         <f t="shared" si="0"/>
-        <v>1.0826875452940836</v>
+        <v>1.0710823554249722</v>
       </c>
       <c r="G41">
         <v>6</v>
@@ -2948,11 +2948,11 @@
         <v>296.57</v>
       </c>
       <c r="E42">
-        <v>259.29399999999998</v>
+        <v>258.83699999999999</v>
       </c>
       <c r="F42" s="1">
         <f t="shared" si="0"/>
-        <v>1.1437595933573472</v>
+        <v>1.1457790037745763</v>
       </c>
       <c r="G42">
         <v>7</v>
@@ -2982,11 +2982,11 @@
         <v>260.19900000000001</v>
       </c>
       <c r="E43">
-        <v>222.44499999999999</v>
+        <v>220.74799999999999</v>
       </c>
       <c r="F43" s="1">
         <f t="shared" si="0"/>
-        <v>1.1697228528400279</v>
+        <v>1.1787150959465091</v>
       </c>
       <c r="G43">
         <v>7</v>
@@ -3016,11 +3016,11 @@
         <v>143.821</v>
       </c>
       <c r="E44">
-        <v>124.212</v>
+        <v>123.393</v>
       </c>
       <c r="F44" s="1">
         <f t="shared" si="0"/>
-        <v>1.157867194795994</v>
+        <v>1.1655523408945403</v>
       </c>
       <c r="G44">
         <v>34</v>
@@ -3050,11 +3050,11 @@
         <v>1086.1300000000001</v>
       </c>
       <c r="E45">
-        <v>2824.69</v>
+        <v>2383.9499999999998</v>
       </c>
       <c r="F45" s="1">
         <f t="shared" si="0"/>
-        <v>0.38451299080607076</v>
+        <v>0.45560099834308615</v>
       </c>
       <c r="G45">
         <v>209</v>
@@ -3084,11 +3084,11 @@
         <v>741.48</v>
       </c>
       <c r="E46">
-        <v>2197.0700000000002</v>
+        <v>1824.05</v>
       </c>
       <c r="F46" s="1">
         <f t="shared" si="0"/>
-        <v>0.337485833405399</v>
+        <v>0.40650201474740277</v>
       </c>
       <c r="G46">
         <v>181</v>
@@ -3118,11 +3118,11 @@
         <v>353.25200000000001</v>
       </c>
       <c r="E47">
-        <v>335.78899999999999</v>
+        <v>370.08699999999999</v>
       </c>
       <c r="F47" s="1">
         <f t="shared" si="0"/>
-        <v>1.0520058727355572</v>
+        <v>0.95451069613361184</v>
       </c>
       <c r="G47">
         <v>55</v>
@@ -3152,11 +3152,11 @@
         <v>131.51900000000001</v>
       </c>
       <c r="E48">
-        <v>99.735799999999998</v>
+        <v>98.803600000000003</v>
       </c>
       <c r="F48" s="1">
         <f t="shared" si="0"/>
-        <v>1.3186739365403397</v>
+        <v>1.3311154654283852</v>
       </c>
       <c r="G48">
         <v>3</v>
@@ -3186,11 +3186,11 @@
         <v>144.58600000000001</v>
       </c>
       <c r="E49">
-        <v>125.956</v>
+        <v>125.583</v>
       </c>
       <c r="F49" s="1">
         <f t="shared" si="0"/>
-        <v>1.147908793546953</v>
+        <v>1.1513182516741918</v>
       </c>
       <c r="G49">
         <v>10</v>
@@ -3220,11 +3220,11 @@
         <v>426.88299999999998</v>
       </c>
       <c r="E50">
-        <v>370.43799999999999</v>
+        <v>378.815</v>
       </c>
       <c r="F50" s="1">
         <f t="shared" si="0"/>
-        <v>1.152373676566659</v>
+        <v>1.1268904346448794</v>
       </c>
       <c r="G50">
         <v>3</v>
@@ -3254,11 +3254,11 @@
         <v>931.48400000000004</v>
       </c>
       <c r="E51">
-        <v>829.19200000000001</v>
+        <v>811.01199999999994</v>
       </c>
       <c r="F51" s="1">
         <f t="shared" si="0"/>
-        <v>1.1233634670860309</v>
+        <v>1.1485452742992706</v>
       </c>
       <c r="G51">
         <v>47</v>
@@ -3288,11 +3288,11 @@
         <v>264.90199999999999</v>
       </c>
       <c r="E52">
-        <v>229.64099999999999</v>
+        <v>228.351</v>
       </c>
       <c r="F52" s="1">
         <f t="shared" si="0"/>
-        <v>1.1535483646213003</v>
+        <v>1.1600649876724867</v>
       </c>
       <c r="G52">
         <v>4</v>
@@ -3322,11 +3322,11 @@
         <v>1930.02</v>
       </c>
       <c r="E53">
-        <v>1614.05</v>
+        <v>1683.81</v>
       </c>
       <c r="F53" s="1">
         <f t="shared" si="0"/>
-        <v>1.1957622130665098</v>
+        <v>1.146221960910079</v>
       </c>
       <c r="G53">
         <v>37</v>
@@ -3356,11 +3356,11 @@
         <v>85.232699999999994</v>
       </c>
       <c r="E54">
-        <v>71.766800000000003</v>
+        <v>71.705299999999994</v>
       </c>
       <c r="F54" s="1">
         <f t="shared" si="0"/>
-        <v>1.1876341149389409</v>
+        <v>1.1886527216258771</v>
       </c>
       <c r="G54">
         <v>3</v>
@@ -3390,11 +3390,11 @@
         <v>448.142</v>
       </c>
       <c r="E55">
-        <v>381.28899999999999</v>
+        <v>385.46600000000001</v>
       </c>
       <c r="F55" s="1">
         <f t="shared" si="0"/>
-        <v>1.1753341953216589</v>
+        <v>1.1625979982670327</v>
       </c>
       <c r="G55">
         <v>5</v>
@@ -3424,11 +3424,11 @@
         <v>297.17500000000001</v>
       </c>
       <c r="E56">
-        <v>266.69</v>
+        <v>261.86500000000001</v>
       </c>
       <c r="F56" s="1">
         <f t="shared" si="0"/>
-        <v>1.1143087479845515</v>
+        <v>1.1348404712351785</v>
       </c>
       <c r="G56">
         <v>15</v>
@@ -3458,11 +3458,11 @@
         <v>170.05</v>
       </c>
       <c r="E57">
-        <v>148.82599999999999</v>
+        <v>148.03899999999999</v>
       </c>
       <c r="F57" s="1">
         <f t="shared" si="0"/>
-        <v>1.1426094902772366</v>
+        <v>1.1486837927843341</v>
       </c>
       <c r="G57">
         <v>11</v>
@@ -3492,11 +3492,11 @@
         <v>136.655</v>
       </c>
       <c r="E58">
-        <v>115.935</v>
+        <v>115.836</v>
       </c>
       <c r="F58" s="1">
         <f t="shared" si="0"/>
-        <v>1.1787208349506189</v>
+        <v>1.1797282364722539</v>
       </c>
       <c r="G58">
         <v>3</v>
@@ -3526,11 +3526,11 @@
         <v>435.88799999999998</v>
       </c>
       <c r="E59">
-        <v>377.74799999999999</v>
+        <v>361.33</v>
       </c>
       <c r="F59" s="1">
         <f t="shared" si="0"/>
-        <v>1.1539121318974555</v>
+        <v>1.2063432319486342</v>
       </c>
       <c r="G59">
         <v>4</v>
@@ -3560,11 +3560,11 @@
         <v>425.91</v>
       </c>
       <c r="E60">
-        <v>378.58</v>
+        <v>381.08300000000003</v>
       </c>
       <c r="F60" s="1">
         <f t="shared" si="0"/>
-        <v>1.1250198108722067</v>
+        <v>1.1176305424277651</v>
       </c>
       <c r="G60">
         <v>5</v>
@@ -3594,11 +3594,11 @@
         <v>392.17599999999999</v>
       </c>
       <c r="E61">
-        <v>353.983</v>
+        <v>359.29399999999998</v>
       </c>
       <c r="F61" s="1">
         <f t="shared" si="0"/>
-        <v>1.1078950119073514</v>
+        <v>1.0915183665744488</v>
       </c>
       <c r="G61">
         <v>20</v>
@@ -3628,11 +3628,11 @@
         <v>176.90299999999999</v>
       </c>
       <c r="E62">
-        <v>153.80099999999999</v>
+        <v>153.28700000000001</v>
       </c>
       <c r="F62" s="1">
         <f t="shared" si="0"/>
-        <v>1.1502070857796765</v>
+        <v>1.1540639454095911</v>
       </c>
       <c r="G62">
         <v>48</v>
@@ -3662,11 +3662,11 @@
         <v>94.919200000000004</v>
       </c>
       <c r="E63">
-        <v>83.528499999999994</v>
+        <v>83.142700000000005</v>
       </c>
       <c r="F63" s="1">
         <f t="shared" si="0"/>
-        <v>1.1363690237463862</v>
+        <v>1.1416420202856052</v>
       </c>
       <c r="G63">
         <v>14</v>
@@ -3696,11 +3696,11 @@
         <v>53.0627</v>
       </c>
       <c r="E64">
-        <v>44.9146</v>
+        <v>44.737000000000002</v>
       </c>
       <c r="F64" s="1">
         <f t="shared" si="0"/>
-        <v>1.181413170772978</v>
+        <v>1.1861032255180275</v>
       </c>
       <c r="G64">
         <v>29</v>
@@ -3730,11 +3730,11 @@
         <v>245.66200000000001</v>
       </c>
       <c r="E65">
-        <v>194.87100000000001</v>
+        <v>191.93799999999999</v>
       </c>
       <c r="F65" s="1">
         <f t="shared" si="0"/>
-        <v>1.2606390894489174</v>
+        <v>1.2799028853067138</v>
       </c>
       <c r="G65">
         <v>3</v>
@@ -3764,11 +3764,11 @@
         <v>82.586699999999993</v>
       </c>
       <c r="E66">
-        <v>67.937600000000003</v>
+        <v>66.7209</v>
       </c>
       <c r="F66" s="1">
         <f t="shared" si="0"/>
-        <v>1.2156258095664254</v>
+        <v>1.2377935549430537</v>
       </c>
       <c r="G66">
         <v>2</v>
@@ -3798,11 +3798,11 @@
         <v>356.37799999999999</v>
       </c>
       <c r="E67">
-        <v>309.56400000000002</v>
+        <v>307.26900000000001</v>
       </c>
       <c r="F67" s="1">
         <f t="shared" ref="F67:F71" si="2">D67/E67</f>
-        <v>1.1512255947073948</v>
+        <v>1.1598241280441566</v>
       </c>
       <c r="G67">
         <v>4</v>
@@ -3832,11 +3832,11 @@
         <v>212.614</v>
       </c>
       <c r="E68">
-        <v>186.274</v>
+        <v>184.62</v>
       </c>
       <c r="F68" s="1">
         <f t="shared" si="2"/>
-        <v>1.1414045975283722</v>
+        <v>1.151630375907269</v>
       </c>
       <c r="G68">
         <v>4</v>
@@ -3866,11 +3866,11 @@
         <v>216.16399999999999</v>
       </c>
       <c r="E69">
-        <v>189.24100000000001</v>
+        <v>186.761</v>
       </c>
       <c r="F69" s="1">
         <f t="shared" si="2"/>
-        <v>1.1422683245174141</v>
+        <v>1.1574365097638157</v>
       </c>
       <c r="G69">
         <v>6</v>
@@ -3900,11 +3900,11 @@
         <v>79.242699999999999</v>
       </c>
       <c r="E70">
-        <v>64.630600000000001</v>
+        <v>64.041799999999995</v>
       </c>
       <c r="F70" s="1">
         <f t="shared" si="2"/>
-        <v>1.2260864048918005</v>
+        <v>1.2373590373787122</v>
       </c>
       <c r="G70">
         <v>11</v>
@@ -3934,11 +3934,11 @@
         <v>167.25899999999999</v>
       </c>
       <c r="E71">
-        <v>143.565</v>
+        <v>142.92400000000001</v>
       </c>
       <c r="F71" s="1">
         <f t="shared" si="2"/>
-        <v>1.1650402256817469</v>
+        <v>1.1702653158321903</v>
       </c>
       <c r="G71">
         <v>11</v>

</xml_diff>

<commit_message>
Updated srlpi results with code alignment and NOP's.
</commit_message>
<xml_diff>
--- a/results/srlpi-ARM.xlsx
+++ b/results/srlpi-ARM.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27907"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28016"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="25220" yWindow="6520" windowWidth="22660" windowHeight="17560" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="6100" yWindow="6780" windowWidth="22660" windowHeight="17560" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="GPCE matrices" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="105">
   <si>
     <t>email-EuAll</t>
   </si>
@@ -337,6 +337,12 @@
   </si>
   <si>
     <t>CSRbyNZ-71f0de</t>
+  </si>
+  <si>
+    <t>CSRbyNZ-4b7631</t>
+  </si>
+  <si>
+    <t>stencil-4b7631</t>
   </si>
 </sst>
 </file>
@@ -403,7 +409,67 @@
     <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="8">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -700,7 +766,7 @@
   <dimension ref="A1:J24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L1" sqref="L1"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -723,7 +789,7 @@
         <v>24</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>96</v>
@@ -755,11 +821,11 @@
         <v>46026.5</v>
       </c>
       <c r="E2">
-        <v>45762.2</v>
+        <v>45093</v>
       </c>
       <c r="F2" s="1">
         <f t="shared" ref="F2:F24" si="0">D2/E2</f>
-        <v>1.0057755090445828</v>
+        <v>1.020701661011687</v>
       </c>
       <c r="G2">
         <v>311</v>
@@ -789,11 +855,11 @@
         <v>27425.5</v>
       </c>
       <c r="E3">
-        <v>32806.400000000001</v>
+        <v>32492.9</v>
       </c>
       <c r="F3" s="1">
         <f t="shared" si="0"/>
-        <v>0.83598017460007801</v>
+        <v>0.84404593003394579</v>
       </c>
       <c r="G3">
         <v>162</v>
@@ -823,11 +889,11 @@
         <v>34805.9</v>
       </c>
       <c r="E4">
-        <v>39503.1</v>
+        <v>39220.300000000003</v>
       </c>
       <c r="F4" s="1">
         <f t="shared" si="0"/>
-        <v>0.88109287625528132</v>
+        <v>0.88744604197316179</v>
       </c>
       <c r="G4">
         <v>326</v>
@@ -857,11 +923,11 @@
         <v>40743.699999999997</v>
       </c>
       <c r="E5">
-        <v>43674.2</v>
+        <v>43263.8</v>
       </c>
       <c r="F5" s="1">
         <f t="shared" si="0"/>
-        <v>0.93290088885428923</v>
+        <v>0.94175037791409899</v>
       </c>
       <c r="G5">
         <v>279</v>
@@ -891,11 +957,11 @@
         <v>87978.2</v>
       </c>
       <c r="E6">
-        <v>93737.4</v>
+        <v>93216.9</v>
       </c>
       <c r="F6" s="1">
         <f t="shared" si="0"/>
-        <v>0.93856027583440549</v>
+        <v>0.94380096313007622</v>
       </c>
       <c r="G6">
         <v>312</v>
@@ -925,11 +991,11 @@
         <v>216464</v>
       </c>
       <c r="E7">
-        <v>234662</v>
+        <v>237339</v>
       </c>
       <c r="F7" s="1">
         <f t="shared" si="0"/>
-        <v>0.92245016236118327</v>
+        <v>0.91204563935973437</v>
       </c>
       <c r="G7">
         <v>370</v>
@@ -959,11 +1025,11 @@
         <v>22222.5</v>
       </c>
       <c r="E8">
-        <v>23595.4</v>
+        <v>23716.3</v>
       </c>
       <c r="F8" s="1">
         <f t="shared" si="0"/>
-        <v>0.9418149300287344</v>
+        <v>0.93701378376896904</v>
       </c>
       <c r="G8">
         <v>25</v>
@@ -993,11 +1059,11 @@
         <v>24999.4</v>
       </c>
       <c r="E9">
-        <v>26264.400000000001</v>
+        <v>26229.1</v>
       </c>
       <c r="F9" s="1">
         <f t="shared" si="0"/>
-        <v>0.95183594523385262</v>
+        <v>0.95311695788265716</v>
       </c>
       <c r="G9">
         <v>22</v>
@@ -1027,11 +1093,11 @@
         <v>29468.9</v>
       </c>
       <c r="E10">
-        <v>30892.6</v>
+        <v>30817</v>
       </c>
       <c r="F10" s="1">
         <f t="shared" si="0"/>
-        <v>0.95391452969319523</v>
+        <v>0.95625466463315711</v>
       </c>
       <c r="G10">
         <v>70</v>
@@ -1061,11 +1127,11 @@
         <v>59540.800000000003</v>
       </c>
       <c r="E11">
-        <v>56036.9</v>
+        <v>56162.9</v>
       </c>
       <c r="F11" s="1">
         <f t="shared" si="0"/>
-        <v>1.0625284410807878</v>
+        <v>1.060144686260859</v>
       </c>
       <c r="G11">
         <v>1</v>
@@ -1095,11 +1161,11 @@
         <v>48752.6</v>
       </c>
       <c r="E12">
-        <v>46687.4</v>
+        <v>47300.6</v>
       </c>
       <c r="F12" s="1">
         <f t="shared" si="0"/>
-        <v>1.0442346328988121</v>
+        <v>1.0306972850238687</v>
       </c>
       <c r="G12">
         <v>3</v>
@@ -1129,11 +1195,11 @@
         <v>42246.3</v>
       </c>
       <c r="E13">
-        <v>44015.3</v>
+        <v>43805.3</v>
       </c>
       <c r="F13" s="1">
         <f t="shared" si="0"/>
-        <v>0.95980942990278384</v>
+        <v>0.96441069916197353</v>
       </c>
       <c r="G13">
         <v>71</v>
@@ -1163,11 +1229,11 @@
         <v>71419.600000000006</v>
       </c>
       <c r="E14">
-        <v>80062.5</v>
+        <v>80133.3</v>
       </c>
       <c r="F14" s="1">
         <f t="shared" si="0"/>
-        <v>0.89204808743169406</v>
+        <v>0.89125993812809412</v>
       </c>
       <c r="G14">
         <v>27</v>
@@ -1197,11 +1263,11 @@
         <v>143862</v>
       </c>
       <c r="E15">
-        <v>171609</v>
+        <v>170468</v>
       </c>
       <c r="F15" s="1">
         <f t="shared" si="0"/>
-        <v>0.83831267590860614</v>
+        <v>0.84392378628246945</v>
       </c>
       <c r="G15">
         <v>22</v>
@@ -1231,11 +1297,11 @@
         <v>79212.600000000006</v>
       </c>
       <c r="E16">
-        <v>97190.1</v>
+        <v>97154.3</v>
       </c>
       <c r="F16" s="1">
         <f t="shared" si="0"/>
-        <v>0.81502745650019914</v>
+        <v>0.81532778271265405</v>
       </c>
       <c r="G16">
         <v>23</v>
@@ -1265,11 +1331,11 @@
         <v>79186.399999999994</v>
       </c>
       <c r="E17">
-        <v>76615.7</v>
+        <v>76988</v>
       </c>
       <c r="F17" s="1">
         <f t="shared" si="0"/>
-        <v>1.033553175132512</v>
+        <v>1.0285550994960253</v>
       </c>
       <c r="G17">
         <v>1</v>
@@ -1299,11 +1365,11 @@
         <v>84754.8</v>
       </c>
       <c r="E18">
-        <v>136559</v>
+        <v>136844</v>
       </c>
       <c r="F18" s="1">
         <f t="shared" si="0"/>
-        <v>0.62064602113372247</v>
+        <v>0.61935342433720153</v>
       </c>
       <c r="G18">
         <v>60</v>
@@ -1333,11 +1399,11 @@
         <v>100704</v>
       </c>
       <c r="E19">
-        <v>110779</v>
+        <v>110296</v>
       </c>
       <c r="F19" s="1">
         <f t="shared" si="0"/>
-        <v>0.90905315989492597</v>
+        <v>0.91303401755276714</v>
       </c>
       <c r="G19">
         <v>28</v>
@@ -1367,11 +1433,11 @@
         <v>170626</v>
       </c>
       <c r="E20">
-        <v>162576</v>
+        <v>163554</v>
       </c>
       <c r="F20" s="1">
         <f t="shared" si="0"/>
-        <v>1.0495153036118492</v>
+        <v>1.0432395416804237</v>
       </c>
       <c r="G20">
         <v>3</v>
@@ -1401,11 +1467,11 @@
         <v>123100</v>
       </c>
       <c r="E21">
-        <v>116919</v>
+        <v>115988</v>
       </c>
       <c r="F21" s="1">
         <f t="shared" si="0"/>
-        <v>1.0528656591315355</v>
+        <v>1.0613166879332345</v>
       </c>
       <c r="G21">
         <v>3</v>
@@ -1435,11 +1501,11 @@
         <v>93398.1</v>
       </c>
       <c r="E22">
-        <v>111296</v>
+        <v>110883</v>
       </c>
       <c r="F22" s="1">
         <f t="shared" si="0"/>
-        <v>0.83918649367452569</v>
+        <v>0.84231216687860178</v>
       </c>
       <c r="G22">
         <v>29</v>
@@ -1469,11 +1535,11 @@
         <v>116283</v>
       </c>
       <c r="E23">
-        <v>165427</v>
+        <v>165656</v>
       </c>
       <c r="F23" s="1">
         <f t="shared" si="0"/>
-        <v>0.70292636631263339</v>
+        <v>0.70195465301588833</v>
       </c>
       <c r="G23">
         <v>147</v>
@@ -1503,11 +1569,11 @@
         <v>196744</v>
       </c>
       <c r="E24">
-        <v>198853</v>
+        <v>198902</v>
       </c>
       <c r="F24" s="1">
         <f t="shared" si="0"/>
-        <v>0.98939417559704912</v>
+        <v>0.98915043589305285</v>
       </c>
       <c r="G24">
         <v>9</v>
@@ -1530,10 +1596,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J71"/>
+  <dimension ref="A1:O71"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L2" sqref="L2"/>
+      <selection activeCell="O2" sqref="O2:O71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1542,7 +1608,7 @@
     <col min="3" max="3" width="8" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>23</v>
       </c>
@@ -1573,8 +1639,17 @@
       <c r="J1" s="2" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K1" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>26</v>
       </c>
@@ -1607,8 +1682,22 @@
       <c r="J2">
         <v>2128</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K2">
+        <v>209.858</v>
+      </c>
+      <c r="L2" s="1">
+        <f>D2/K2</f>
+        <v>1.2504693649991898</v>
+      </c>
+      <c r="N2">
+        <v>231.87</v>
+      </c>
+      <c r="O2" s="1">
+        <f>E2/N2</f>
+        <v>0.99823176780092293</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>27</v>
       </c>
@@ -1641,8 +1730,22 @@
       <c r="J3">
         <v>3941</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K3">
+        <v>900.02599999999995</v>
+      </c>
+      <c r="L3" s="1">
+        <f>D3/K3</f>
+        <v>0.49600344878925723</v>
+      </c>
+      <c r="N3">
+        <v>416.44</v>
+      </c>
+      <c r="O3" s="1">
+        <f>E3/N3</f>
+        <v>1.0157981942176544</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>28</v>
       </c>
@@ -1675,8 +1778,22 @@
       <c r="J4">
         <v>1812</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K4">
+        <v>325.65899999999999</v>
+      </c>
+      <c r="L4" s="1">
+        <f>D4/K4</f>
+        <v>0.83708725998667322</v>
+      </c>
+      <c r="N4">
+        <v>246.54400000000001</v>
+      </c>
+      <c r="O4" s="1">
+        <f>E4/N4</f>
+        <v>0.99199331559478221</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>29</v>
       </c>
@@ -1709,8 +1826,22 @@
       <c r="J5">
         <v>5470</v>
       </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K5">
+        <v>1060.48</v>
+      </c>
+      <c r="L5" s="1">
+        <f>D5/K5</f>
+        <v>0.45699305974652987</v>
+      </c>
+      <c r="N5">
+        <v>363.19299999999998</v>
+      </c>
+      <c r="O5" s="1">
+        <f>E5/N5</f>
+        <v>1.0080480626003254</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>30</v>
       </c>
@@ -1743,8 +1874,22 @@
       <c r="J6">
         <v>3083</v>
       </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K6">
+        <v>225.077</v>
+      </c>
+      <c r="L6" s="1">
+        <f>D6/K6</f>
+        <v>1.1590788930010618</v>
+      </c>
+      <c r="N6">
+        <v>224.393</v>
+      </c>
+      <c r="O6" s="1">
+        <f>E6/N6</f>
+        <v>0.99646156520034046</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>31</v>
       </c>
@@ -1777,8 +1922,22 @@
       <c r="J7">
         <v>565</v>
       </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K7">
+        <v>66.472999999999999</v>
+      </c>
+      <c r="L7" s="1">
+        <f>D7/K7</f>
+        <v>1.437478374678441</v>
+      </c>
+      <c r="N7">
+        <v>74.936199999999999</v>
+      </c>
+      <c r="O7" s="1">
+        <f>E7/N7</f>
+        <v>1.0011649910190268</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>32</v>
       </c>
@@ -1811,8 +1970,22 @@
       <c r="J8">
         <v>637</v>
       </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K8">
+        <v>76.375399999999999</v>
+      </c>
+      <c r="L8" s="1">
+        <f>D8/K8</f>
+        <v>1.418742160433857</v>
+      </c>
+      <c r="N8">
+        <v>85.340299999999999</v>
+      </c>
+      <c r="O8" s="1">
+        <f>E8/N8</f>
+        <v>1.0008753191633966</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>33</v>
       </c>
@@ -1845,8 +2018,22 @@
       <c r="J9">
         <v>75</v>
       </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K9">
+        <v>48.409500000000001</v>
+      </c>
+      <c r="L9" s="1">
+        <f>D9/K9</f>
+        <v>1.4057075574009232</v>
+      </c>
+      <c r="N9">
+        <v>57.669899999999998</v>
+      </c>
+      <c r="O9" s="1">
+        <f>E9/N9</f>
+        <v>0.99917114473928348</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>34</v>
       </c>
@@ -1879,8 +2066,22 @@
       <c r="J10">
         <v>1664</v>
       </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K10">
+        <v>951.61900000000003</v>
+      </c>
+      <c r="L10" s="1">
+        <f>D10/K10</f>
+        <v>0.53146479841196947</v>
+      </c>
+      <c r="N10">
+        <v>603.63800000000003</v>
+      </c>
+      <c r="O10" s="1">
+        <f>E10/N10</f>
+        <v>0.86163561604802874</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>35</v>
       </c>
@@ -1913,8 +2114,22 @@
       <c r="J11">
         <v>240</v>
       </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K11">
+        <v>53.899000000000001</v>
+      </c>
+      <c r="L11" s="1">
+        <f>D11/K11</f>
+        <v>1.4235124955936103</v>
+      </c>
+      <c r="N11">
+        <v>63.706800000000001</v>
+      </c>
+      <c r="O11" s="1">
+        <f>E11/N11</f>
+        <v>1.0005493919016495</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>36</v>
       </c>
@@ -1947,8 +2162,22 @@
       <c r="J12">
         <v>1297</v>
       </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K12">
+        <v>223.577</v>
+      </c>
+      <c r="L12" s="1">
+        <f>D12/K12</f>
+        <v>1.2858165195883298</v>
+      </c>
+      <c r="N12">
+        <v>260.572</v>
+      </c>
+      <c r="O12" s="1">
+        <f>E12/N12</f>
+        <v>1.0004221481970434</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>37</v>
       </c>
@@ -1981,8 +2210,22 @@
       <c r="J13">
         <v>328</v>
       </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K13">
+        <v>41.668199999999999</v>
+      </c>
+      <c r="L13" s="1">
+        <f>D13/K13</f>
+        <v>1.4351807853470993</v>
+      </c>
+      <c r="N13">
+        <v>50.942799999999998</v>
+      </c>
+      <c r="O13" s="1">
+        <f>E13/N13</f>
+        <v>1.0013740901560182</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>38</v>
       </c>
@@ -2015,8 +2258,22 @@
       <c r="J14">
         <v>240</v>
       </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K14">
+        <v>136.72</v>
+      </c>
+      <c r="L14" s="1">
+        <f>D14/K14</f>
+        <v>1.335649502633119</v>
+      </c>
+      <c r="N14">
+        <v>155.10900000000001</v>
+      </c>
+      <c r="O14" s="1">
+        <f>E14/N14</f>
+        <v>0.99730512091496948</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>39</v>
       </c>
@@ -2049,8 +2306,22 @@
       <c r="J15">
         <v>808</v>
       </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K15">
+        <v>65.062799999999996</v>
+      </c>
+      <c r="L15" s="1">
+        <f>D15/K15</f>
+        <v>1.4356944367595617</v>
+      </c>
+      <c r="N15">
+        <v>78.149600000000007</v>
+      </c>
+      <c r="O15" s="1">
+        <f>E15/N15</f>
+        <v>1.003160604788764</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>40</v>
       </c>
@@ -2083,8 +2354,22 @@
       <c r="J16">
         <v>860</v>
       </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K16">
+        <v>140.084</v>
+      </c>
+      <c r="L16" s="1">
+        <f>D16/K16</f>
+        <v>1.3413166385882755</v>
+      </c>
+      <c r="N16">
+        <v>157.227</v>
+      </c>
+      <c r="O16" s="1">
+        <f>E16/N16</f>
+        <v>1.0052471903680664</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>41</v>
       </c>
@@ -2117,8 +2402,22 @@
       <c r="J17">
         <v>3524</v>
       </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K17">
+        <v>648.06899999999996</v>
+      </c>
+      <c r="L17" s="1">
+        <f>D17/K17</f>
+        <v>0.65761979048527242</v>
+      </c>
+      <c r="N17">
+        <v>347.21199999999999</v>
+      </c>
+      <c r="O17" s="1">
+        <f>E17/N17</f>
+        <v>1.0382561662615348</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>42</v>
       </c>
@@ -2151,8 +2450,22 @@
       <c r="J18">
         <v>952</v>
       </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K18">
+        <v>89.675700000000006</v>
+      </c>
+      <c r="L18" s="1">
+        <f>D18/K18</f>
+        <v>1.4265514515080451</v>
+      </c>
+      <c r="N18">
+        <v>109.892</v>
+      </c>
+      <c r="O18" s="1">
+        <f>E18/N18</f>
+        <v>1.0049412150111019</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>43</v>
       </c>
@@ -2185,8 +2498,22 @@
       <c r="J19">
         <v>232</v>
       </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K19">
+        <v>50.402900000000002</v>
+      </c>
+      <c r="L19" s="1">
+        <f>D19/K19</f>
+        <v>1.4275924599576613</v>
+      </c>
+      <c r="N19">
+        <v>60.027200000000001</v>
+      </c>
+      <c r="O19" s="1">
+        <f>E19/N19</f>
+        <v>1.0077098382066796</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>44</v>
       </c>
@@ -2219,8 +2546,22 @@
       <c r="J20">
         <v>395</v>
       </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K20">
+        <v>510.80500000000001</v>
+      </c>
+      <c r="L20" s="1">
+        <f>D20/K20</f>
+        <v>0.95405095878074808</v>
+      </c>
+      <c r="N20">
+        <v>480.55399999999997</v>
+      </c>
+      <c r="O20" s="1">
+        <f>E20/N20</f>
+        <v>1.0848104479413343</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>45</v>
       </c>
@@ -2253,8 +2594,22 @@
       <c r="J21">
         <v>9</v>
       </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K21">
+        <v>66.117599999999996</v>
+      </c>
+      <c r="L21" s="1">
+        <f>D21/K21</f>
+        <v>1.3704096942417754</v>
+      </c>
+      <c r="N21">
+        <v>77.048599999999993</v>
+      </c>
+      <c r="O21" s="1">
+        <f>E21/N21</f>
+        <v>0.99755608797564133</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>46</v>
       </c>
@@ -2287,8 +2642,22 @@
       <c r="J22">
         <v>38</v>
       </c>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K22">
+        <v>51.446899999999999</v>
+      </c>
+      <c r="L22" s="1">
+        <f>D22/K22</f>
+        <v>1.3771228198394849</v>
+      </c>
+      <c r="N22">
+        <v>59.622300000000003</v>
+      </c>
+      <c r="O22" s="1">
+        <f>E22/N22</f>
+        <v>0.99765523973412629</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>47</v>
       </c>
@@ -2321,8 +2690,22 @@
       <c r="J23">
         <v>1015</v>
       </c>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K23">
+        <v>266.233</v>
+      </c>
+      <c r="L23" s="1">
+        <f>D23/K23</f>
+        <v>1.1675524822242171</v>
+      </c>
+      <c r="N23">
+        <v>286.63900000000001</v>
+      </c>
+      <c r="O23" s="1">
+        <f>E23/N23</f>
+        <v>1.0039038651404728</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>48</v>
       </c>
@@ -2355,8 +2738,22 @@
       <c r="J24">
         <v>12</v>
       </c>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K24">
+        <v>1043.5999999999999</v>
+      </c>
+      <c r="L24" s="1">
+        <f>D24/K24</f>
+        <v>1.8954197010348794</v>
+      </c>
+      <c r="N24">
+        <v>1849.25</v>
+      </c>
+      <c r="O24" s="1">
+        <f>E24/N24</f>
+        <v>0.99730160876030827</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>49</v>
       </c>
@@ -2389,8 +2786,22 @@
       <c r="J25">
         <v>18</v>
       </c>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K25">
+        <v>146.66</v>
+      </c>
+      <c r="L25" s="1">
+        <f>D25/K25</f>
+        <v>1.3691735987999454</v>
+      </c>
+      <c r="N25">
+        <v>170.76599999999999</v>
+      </c>
+      <c r="O25" s="1">
+        <f>E25/N25</f>
+        <v>1.003109518288184</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>50</v>
       </c>
@@ -2423,8 +2834,22 @@
       <c r="J26">
         <v>355</v>
       </c>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K26">
+        <v>85.430400000000006</v>
+      </c>
+      <c r="L26" s="1">
+        <f>D26/K26</f>
+        <v>1.3760324193729632</v>
+      </c>
+      <c r="N26">
+        <v>99.241100000000003</v>
+      </c>
+      <c r="O26" s="1">
+        <f>E26/N26</f>
+        <v>1.0036517128488096</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>51</v>
       </c>
@@ -2457,8 +2882,22 @@
       <c r="J27">
         <v>963</v>
       </c>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K27">
+        <v>212.512</v>
+      </c>
+      <c r="L27" s="1">
+        <f>D27/K27</f>
+        <v>1.3104530567685591</v>
+      </c>
+      <c r="N27">
+        <v>248.27699999999999</v>
+      </c>
+      <c r="O27" s="1">
+        <f>E27/N27</f>
+        <v>1.002481099739404</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>52</v>
       </c>
@@ -2491,8 +2930,22 @@
       <c r="J28">
         <v>187</v>
       </c>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K28">
+        <v>26.026299999999999</v>
+      </c>
+      <c r="L28" s="1">
+        <f>D28/K28</f>
+        <v>1.4295001594540906</v>
+      </c>
+      <c r="N28">
+        <v>28.1645</v>
+      </c>
+      <c r="O28" s="1">
+        <f>E28/N28</f>
+        <v>0.99783770349198453</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>53</v>
       </c>
@@ -2525,8 +2978,22 @@
       <c r="J29">
         <v>151</v>
       </c>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K29">
+        <v>61.848599999999998</v>
+      </c>
+      <c r="L29" s="1">
+        <f>D29/K29</f>
+        <v>1.3476085149865964</v>
+      </c>
+      <c r="N29">
+        <v>75.424499999999995</v>
+      </c>
+      <c r="O29" s="1">
+        <f>E29/N29</f>
+        <v>1.0005130958773343</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>54</v>
       </c>
@@ -2559,8 +3026,22 @@
       <c r="J30">
         <v>1066</v>
       </c>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K30">
+        <v>78.309899999999999</v>
+      </c>
+      <c r="L30" s="1">
+        <f>D30/K30</f>
+        <v>1.4454621957121641</v>
+      </c>
+      <c r="N30">
+        <v>93.876800000000003</v>
+      </c>
+      <c r="O30" s="1">
+        <f>E30/N30</f>
+        <v>1.010028036746033</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>55</v>
       </c>
@@ -2593,8 +3074,22 @@
       <c r="J31">
         <v>710</v>
       </c>
-    </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K31">
+        <v>130.869</v>
+      </c>
+      <c r="L31" s="1">
+        <f>D31/K31</f>
+        <v>2.4517647418410777</v>
+      </c>
+      <c r="N31">
+        <v>140.029</v>
+      </c>
+      <c r="O31" s="1">
+        <f>E31/N31</f>
+        <v>1.013754293753437</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>56</v>
       </c>
@@ -2627,8 +3122,22 @@
       <c r="J32">
         <v>436</v>
       </c>
-    </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K32">
+        <v>474.178</v>
+      </c>
+      <c r="L32" s="1">
+        <f>D32/K32</f>
+        <v>0.80028596856032974</v>
+      </c>
+      <c r="N32">
+        <v>364.065</v>
+      </c>
+      <c r="O32" s="1">
+        <f>E32/N32</f>
+        <v>0.98671391097743533</v>
+      </c>
+    </row>
+    <row r="33" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>57</v>
       </c>
@@ -2661,8 +3170,22 @@
       <c r="J33">
         <v>1138</v>
       </c>
-    </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K33">
+        <v>87.902900000000002</v>
+      </c>
+      <c r="L33" s="1">
+        <f>D33/K33</f>
+        <v>1.3624578938806342</v>
+      </c>
+      <c r="N33">
+        <v>101.10899999999999</v>
+      </c>
+      <c r="O33" s="1">
+        <f>E33/N33</f>
+        <v>1.0002472579097805</v>
+      </c>
+    </row>
+    <row r="34" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>58</v>
       </c>
@@ -2695,8 +3218,22 @@
       <c r="J34">
         <v>99</v>
       </c>
-    </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K34">
+        <v>74.308800000000005</v>
+      </c>
+      <c r="L34" s="1">
+        <f>D34/K34</f>
+        <v>1.3539177055745752</v>
+      </c>
+      <c r="N34">
+        <v>87.426199999999994</v>
+      </c>
+      <c r="O34" s="1">
+        <f>E34/N34</f>
+        <v>1.0045226716933826</v>
+      </c>
+    </row>
+    <row r="35" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>59</v>
       </c>
@@ -2729,8 +3266,22 @@
       <c r="J35">
         <v>8</v>
       </c>
-    </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K35">
+        <v>83.962900000000005</v>
+      </c>
+      <c r="L35" s="1">
+        <f>D35/K35</f>
+        <v>1.3840874957868297</v>
+      </c>
+      <c r="N35">
+        <v>92.071299999999994</v>
+      </c>
+      <c r="O35" s="1">
+        <f>E35/N35</f>
+        <v>1.0000130333773936</v>
+      </c>
+    </row>
+    <row r="36" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>60</v>
       </c>
@@ -2763,8 +3314,22 @@
       <c r="J36">
         <v>1455</v>
       </c>
-    </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K36">
+        <v>116.22199999999999</v>
+      </c>
+      <c r="L36" s="1">
+        <f>D36/K36</f>
+        <v>1.4111613980141455</v>
+      </c>
+      <c r="N36">
+        <v>139.32</v>
+      </c>
+      <c r="O36" s="1">
+        <f>E36/N36</f>
+        <v>1.0003301751363769</v>
+      </c>
+    </row>
+    <row r="37" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>61</v>
       </c>
@@ -2797,8 +3362,22 @@
       <c r="J37">
         <v>5</v>
       </c>
-    </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K37">
+        <v>60.330300000000001</v>
+      </c>
+      <c r="L37" s="1">
+        <f>D37/K37</f>
+        <v>1.3925241545293161</v>
+      </c>
+      <c r="N37">
+        <v>70.623599999999996</v>
+      </c>
+      <c r="O37" s="1">
+        <f>E37/N37</f>
+        <v>0.99032759587446695</v>
+      </c>
+    </row>
+    <row r="38" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>62</v>
       </c>
@@ -2831,8 +3410,22 @@
       <c r="J38">
         <v>905</v>
       </c>
-    </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K38">
+        <v>79.621499999999997</v>
+      </c>
+      <c r="L38" s="1">
+        <f>D38/K38</f>
+        <v>1.4187876390170997</v>
+      </c>
+      <c r="N38">
+        <v>95.056299999999993</v>
+      </c>
+      <c r="O38" s="1">
+        <f>E38/N38</f>
+        <v>1.0047876889801097</v>
+      </c>
+    </row>
+    <row r="39" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>63</v>
       </c>
@@ -2865,8 +3458,22 @@
       <c r="J39">
         <v>409</v>
       </c>
-    </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K39">
+        <v>47.173200000000001</v>
+      </c>
+      <c r="L39" s="1">
+        <f>D39/K39</f>
+        <v>1.4483287120653252</v>
+      </c>
+      <c r="N39">
+        <v>58.728700000000003</v>
+      </c>
+      <c r="O39" s="1">
+        <f>E39/N39</f>
+        <v>1.0045429236472116</v>
+      </c>
+    </row>
+    <row r="40" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>64</v>
       </c>
@@ -2899,8 +3506,22 @@
       <c r="J40">
         <v>847</v>
       </c>
-    </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K40">
+        <v>78.252499999999998</v>
+      </c>
+      <c r="L40" s="1">
+        <f>D40/K40</f>
+        <v>1.471339573815533</v>
+      </c>
+      <c r="N40">
+        <v>97.980900000000005</v>
+      </c>
+      <c r="O40" s="1">
+        <f>E40/N40</f>
+        <v>0.99970300334044693</v>
+      </c>
+    </row>
+    <row r="41" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>65</v>
       </c>
@@ -2933,8 +3554,22 @@
       <c r="J41">
         <v>61</v>
       </c>
-    </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K41">
+        <v>390.93</v>
+      </c>
+      <c r="L41" s="1">
+        <f>D41/K41</f>
+        <v>1.2458342925843502</v>
+      </c>
+      <c r="N41">
+        <v>522.62400000000002</v>
+      </c>
+      <c r="O41" s="1">
+        <f>E41/N41</f>
+        <v>0.87005571883419053</v>
+      </c>
+    </row>
+    <row r="42" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>66</v>
       </c>
@@ -2967,8 +3602,22 @@
       <c r="J42">
         <v>380</v>
       </c>
-    </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K42">
+        <v>234.46600000000001</v>
+      </c>
+      <c r="L42" s="1">
+        <f>D42/K42</f>
+        <v>1.2648742248343043</v>
+      </c>
+      <c r="N42">
+        <v>256.16399999999999</v>
+      </c>
+      <c r="O42" s="1">
+        <f>E42/N42</f>
+        <v>1.0104347215065348</v>
+      </c>
+    </row>
+    <row r="43" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>67</v>
       </c>
@@ -3001,8 +3650,22 @@
       <c r="J43">
         <v>74</v>
       </c>
-    </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K43">
+        <v>198.673</v>
+      </c>
+      <c r="L43" s="1">
+        <f>D43/K43</f>
+        <v>1.309684758371797</v>
+      </c>
+      <c r="N43">
+        <v>219.917</v>
+      </c>
+      <c r="O43" s="1">
+        <f>E43/N43</f>
+        <v>1.003778698327096</v>
+      </c>
+    </row>
+    <row r="44" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>68</v>
       </c>
@@ -3035,8 +3698,22 @@
       <c r="J44">
         <v>597</v>
       </c>
-    </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K44">
+        <v>103.26600000000001</v>
+      </c>
+      <c r="L44" s="1">
+        <f>D44/K44</f>
+        <v>1.3927236457304437</v>
+      </c>
+      <c r="N44">
+        <v>123.44199999999999</v>
+      </c>
+      <c r="O44" s="1">
+        <f>E44/N44</f>
+        <v>0.99960305244568304</v>
+      </c>
+    </row>
+    <row r="45" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>69</v>
       </c>
@@ -3069,8 +3746,22 @@
       <c r="J45">
         <v>445</v>
       </c>
-    </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K45">
+        <v>1672.65</v>
+      </c>
+      <c r="L45" s="1">
+        <f>D45/K45</f>
+        <v>0.64934684482707083</v>
+      </c>
+      <c r="N45">
+        <v>2364.88</v>
+      </c>
+      <c r="O45" s="1">
+        <f>E45/N45</f>
+        <v>1.0080638341057473</v>
+      </c>
+    </row>
+    <row r="46" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>70</v>
       </c>
@@ -3103,8 +3794,22 @@
       <c r="J46">
         <v>436</v>
       </c>
-    </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K46">
+        <v>1265.22</v>
+      </c>
+      <c r="L46" s="1">
+        <f>D46/K46</f>
+        <v>0.58604827618912125</v>
+      </c>
+      <c r="N46">
+        <v>1831.84</v>
+      </c>
+      <c r="O46" s="1">
+        <f>E46/N46</f>
+        <v>0.99574744519171987</v>
+      </c>
+    </row>
+    <row r="47" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>71</v>
       </c>
@@ -3137,8 +3842,22 @@
       <c r="J47">
         <v>346</v>
       </c>
-    </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K47">
+        <v>304.75599999999997</v>
+      </c>
+      <c r="L47" s="1">
+        <f>D47/K47</f>
+        <v>1.1591305831550487</v>
+      </c>
+      <c r="N47">
+        <v>383.41300000000001</v>
+      </c>
+      <c r="O47" s="1">
+        <f>E47/N47</f>
+        <v>0.96524374499560517</v>
+      </c>
+    </row>
+    <row r="48" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>72</v>
       </c>
@@ -3171,8 +3890,22 @@
       <c r="J48">
         <v>551</v>
       </c>
-    </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K48">
+        <v>108.973</v>
+      </c>
+      <c r="L48" s="1">
+        <f>D48/K48</f>
+        <v>1.2068952859882724</v>
+      </c>
+      <c r="N48">
+        <v>98.622699999999995</v>
+      </c>
+      <c r="O48" s="1">
+        <f>E48/N48</f>
+        <v>1.0018342633085486</v>
+      </c>
+    </row>
+    <row r="49" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>73</v>
       </c>
@@ -3205,8 +3938,22 @@
       <c r="J49">
         <v>24</v>
       </c>
-    </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K49">
+        <v>105.742</v>
+      </c>
+      <c r="L49" s="1">
+        <f>D49/K49</f>
+        <v>1.3673469387755102</v>
+      </c>
+      <c r="N49">
+        <v>126.59399999999999</v>
+      </c>
+      <c r="O49" s="1">
+        <f>E49/N49</f>
+        <v>0.99201383951846067</v>
+      </c>
+    </row>
+    <row r="50" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>74</v>
       </c>
@@ -3239,8 +3986,22 @@
       <c r="J50">
         <v>4</v>
       </c>
-    </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K50">
+        <v>330.166</v>
+      </c>
+      <c r="L50" s="1">
+        <f>D50/K50</f>
+        <v>1.2929344632699915</v>
+      </c>
+      <c r="N50">
+        <v>370.435</v>
+      </c>
+      <c r="O50" s="1">
+        <f>E50/N50</f>
+        <v>1.0226220524518472</v>
+      </c>
+    </row>
+    <row r="51" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>75</v>
       </c>
@@ -3273,8 +4034,22 @@
       <c r="J51">
         <v>9503</v>
       </c>
-    </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K51">
+        <v>2544.31</v>
+      </c>
+      <c r="L51" s="1">
+        <f>D51/K51</f>
+        <v>0.36610475924710434</v>
+      </c>
+      <c r="N51">
+        <v>813.01300000000003</v>
+      </c>
+      <c r="O51" s="1">
+        <f>E51/N51</f>
+        <v>0.99753878474267932</v>
+      </c>
+    </row>
+    <row r="52" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>76</v>
       </c>
@@ -3307,8 +4082,22 @@
       <c r="J52">
         <v>27</v>
       </c>
-    </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K52">
+        <v>198.28800000000001</v>
+      </c>
+      <c r="L52" s="1">
+        <f>D52/K52</f>
+        <v>1.335945695150488</v>
+      </c>
+      <c r="N52">
+        <v>228.15299999999999</v>
+      </c>
+      <c r="O52" s="1">
+        <f>E52/N52</f>
+        <v>1.0008678386871968</v>
+      </c>
+    </row>
+    <row r="53" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>77</v>
       </c>
@@ -3341,8 +4130,22 @@
       <c r="J53">
         <v>4903</v>
       </c>
-    </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K53">
+        <v>2967.27</v>
+      </c>
+      <c r="L53" s="1">
+        <f>D53/K53</f>
+        <v>0.65043625959215035</v>
+      </c>
+      <c r="N53">
+        <v>1670.33</v>
+      </c>
+      <c r="O53" s="1">
+        <f>E53/N53</f>
+        <v>1.0080702615650801</v>
+      </c>
+    </row>
+    <row r="54" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>78</v>
       </c>
@@ -3375,8 +4178,22 @@
       <c r="J54">
         <v>9</v>
       </c>
-    </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K54">
+        <v>61.112299999999998</v>
+      </c>
+      <c r="L54" s="1">
+        <f>D54/K54</f>
+        <v>1.3946897760352661</v>
+      </c>
+      <c r="N54">
+        <v>71.433300000000003</v>
+      </c>
+      <c r="O54" s="1">
+        <f>E54/N54</f>
+        <v>1.003807747927087</v>
+      </c>
+    </row>
+    <row r="55" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>79</v>
       </c>
@@ -3409,8 +4226,22 @@
       <c r="J55">
         <v>683</v>
       </c>
-    </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K55">
+        <v>414.45</v>
+      </c>
+      <c r="L55" s="1">
+        <f>D55/K55</f>
+        <v>1.081293280250935</v>
+      </c>
+      <c r="N55">
+        <v>375.541</v>
+      </c>
+      <c r="O55" s="1">
+        <f>E55/N55</f>
+        <v>1.0264285390942667</v>
+      </c>
+    </row>
+    <row r="56" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>80</v>
       </c>
@@ -3443,8 +4274,22 @@
       <c r="J56">
         <v>407</v>
       </c>
-    </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K56">
+        <v>218.09700000000001</v>
+      </c>
+      <c r="L56" s="1">
+        <f>D56/K56</f>
+        <v>1.3625817870030308</v>
+      </c>
+      <c r="N56">
+        <v>263.666</v>
+      </c>
+      <c r="O56" s="1">
+        <f>E56/N56</f>
+        <v>0.99316938854459813</v>
+      </c>
+    </row>
+    <row r="57" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>81</v>
       </c>
@@ -3477,8 +4322,22 @@
       <c r="J57">
         <v>467</v>
       </c>
-    </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K57">
+        <v>127.18600000000001</v>
+      </c>
+      <c r="L57" s="1">
+        <f>D57/K57</f>
+        <v>1.3370182252763669</v>
+      </c>
+      <c r="N57">
+        <v>148.226</v>
+      </c>
+      <c r="O57" s="1">
+        <f>E57/N57</f>
+        <v>0.99873841296398735</v>
+      </c>
+    </row>
+    <row r="58" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>82</v>
       </c>
@@ -3511,8 +4370,22 @@
       <c r="J58">
         <v>18</v>
       </c>
-    </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K58">
+        <v>101.066</v>
+      </c>
+      <c r="L58" s="1">
+        <f>D58/K58</f>
+        <v>1.352136227811529</v>
+      </c>
+      <c r="N58">
+        <v>115.34399999999999</v>
+      </c>
+      <c r="O58" s="1">
+        <f>E58/N58</f>
+        <v>1.0042655014565127</v>
+      </c>
+    </row>
+    <row r="59" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>83</v>
       </c>
@@ -3545,8 +4418,22 @@
       <c r="J59">
         <v>397</v>
       </c>
-    </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K59">
+        <v>314.92599999999999</v>
+      </c>
+      <c r="L59" s="1">
+        <f>D59/K59</f>
+        <v>1.3840965814191271</v>
+      </c>
+      <c r="N59">
+        <v>357.226</v>
+      </c>
+      <c r="O59" s="1">
+        <f>E59/N59</f>
+        <v>1.0114885254712702</v>
+      </c>
+    </row>
+    <row r="60" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>84</v>
       </c>
@@ -3579,8 +4466,22 @@
       <c r="J60">
         <v>34</v>
       </c>
-    </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K60">
+        <v>331.702</v>
+      </c>
+      <c r="L60" s="1">
+        <f>D60/K60</f>
+        <v>1.2840139643414874</v>
+      </c>
+      <c r="N60">
+        <v>375.55500000000001</v>
+      </c>
+      <c r="O60" s="1">
+        <f>E60/N60</f>
+        <v>1.0147195484016989</v>
+      </c>
+    </row>
+    <row r="61" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>85</v>
       </c>
@@ -3613,8 +4514,22 @@
       <c r="J61">
         <v>140</v>
       </c>
-    </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K61">
+        <v>305.56</v>
+      </c>
+      <c r="L61" s="1">
+        <f>D61/K61</f>
+        <v>1.2834664223065846</v>
+      </c>
+      <c r="N61">
+        <v>354.63099999999997</v>
+      </c>
+      <c r="O61" s="1">
+        <f>E61/N61</f>
+        <v>1.013148878693628</v>
+      </c>
+    </row>
+    <row r="62" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>86</v>
       </c>
@@ -3647,8 +4562,22 @@
       <c r="J62">
         <v>326</v>
       </c>
-    </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K62">
+        <v>129.19200000000001</v>
+      </c>
+      <c r="L62" s="1">
+        <f>D62/K62</f>
+        <v>1.369303052820608</v>
+      </c>
+      <c r="N62">
+        <v>152.017</v>
+      </c>
+      <c r="O62" s="1">
+        <f>E62/N62</f>
+        <v>1.0083543287921746</v>
+      </c>
+    </row>
+    <row r="63" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>87</v>
       </c>
@@ -3681,8 +4610,22 @@
       <c r="J63">
         <v>273</v>
       </c>
-    </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K63">
+        <v>69.610399999999998</v>
+      </c>
+      <c r="L63" s="1">
+        <f>D63/K63</f>
+        <v>1.3635778561824097</v>
+      </c>
+      <c r="N63">
+        <v>82.674099999999996</v>
+      </c>
+      <c r="O63" s="1">
+        <f>E63/N63</f>
+        <v>1.005668038720712</v>
+      </c>
+    </row>
+    <row r="64" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>88</v>
       </c>
@@ -3715,8 +4658,22 @@
       <c r="J64">
         <v>347</v>
       </c>
-    </row>
-    <row r="65" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K64">
+        <v>36.9238</v>
+      </c>
+      <c r="L64" s="1">
+        <f>D64/K64</f>
+        <v>1.437086648719796</v>
+      </c>
+      <c r="N64">
+        <v>44.590800000000002</v>
+      </c>
+      <c r="O64" s="1">
+        <f>E64/N64</f>
+        <v>1.0032787032302628</v>
+      </c>
+    </row>
+    <row r="65" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>89</v>
       </c>
@@ -3749,8 +4706,22 @@
       <c r="J65">
         <v>22</v>
       </c>
-    </row>
-    <row r="66" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K65">
+        <v>190.68700000000001</v>
+      </c>
+      <c r="L65" s="1">
+        <f>D65/K65</f>
+        <v>1.2882996743354291</v>
+      </c>
+      <c r="N65">
+        <v>191.11500000000001</v>
+      </c>
+      <c r="O65" s="1">
+        <f>E65/N65</f>
+        <v>1.0043063077204823</v>
+      </c>
+    </row>
+    <row r="66" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>90</v>
       </c>
@@ -3783,8 +4754,22 @@
       <c r="J66">
         <v>6</v>
       </c>
-    </row>
-    <row r="67" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K66">
+        <v>60.375</v>
+      </c>
+      <c r="L66" s="1">
+        <f>D66/K66</f>
+        <v>1.367895652173913</v>
+      </c>
+      <c r="N66">
+        <v>66.722700000000003</v>
+      </c>
+      <c r="O66" s="1">
+        <f>E66/N66</f>
+        <v>0.9999730226744421</v>
+      </c>
+    </row>
+    <row r="67" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>91</v>
       </c>
@@ -3817,8 +4802,22 @@
       <c r="J67">
         <v>49</v>
       </c>
-    </row>
-    <row r="68" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K67">
+        <v>268.613</v>
+      </c>
+      <c r="L67" s="1">
+        <f>D67/K67</f>
+        <v>1.326734000215924</v>
+      </c>
+      <c r="N67">
+        <v>308.85700000000003</v>
+      </c>
+      <c r="O67" s="1">
+        <f>E67/N67</f>
+        <v>0.99485846200668915</v>
+      </c>
+    </row>
+    <row r="68" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>92</v>
       </c>
@@ -3851,8 +4850,22 @@
       <c r="J68">
         <v>10</v>
       </c>
-    </row>
-    <row r="69" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K68">
+        <v>160.16300000000001</v>
+      </c>
+      <c r="L68" s="1">
+        <f>D68/K68</f>
+        <v>1.3274851245293857</v>
+      </c>
+      <c r="N68">
+        <v>185.36199999999999</v>
+      </c>
+      <c r="O68" s="1">
+        <f>E68/N68</f>
+        <v>0.99599702204335305</v>
+      </c>
+    </row>
+    <row r="69" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>93</v>
       </c>
@@ -3885,8 +4898,22 @@
       <c r="J69">
         <v>74</v>
       </c>
-    </row>
-    <row r="70" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K69">
+        <v>163.78700000000001</v>
+      </c>
+      <c r="L69" s="1">
+        <f>D69/K69</f>
+        <v>1.3197872847051353</v>
+      </c>
+      <c r="N69">
+        <v>186.01900000000001</v>
+      </c>
+      <c r="O69" s="1">
+        <f>E69/N69</f>
+        <v>1.0039888398496928</v>
+      </c>
+    </row>
+    <row r="70" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>94</v>
       </c>
@@ -3919,8 +4946,22 @@
       <c r="J70">
         <v>799</v>
       </c>
-    </row>
-    <row r="71" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K70">
+        <v>54.655799999999999</v>
+      </c>
+      <c r="L70" s="1">
+        <f>D70/K70</f>
+        <v>1.4498497872137999</v>
+      </c>
+      <c r="N70">
+        <v>63.326000000000001</v>
+      </c>
+      <c r="O70" s="1">
+        <f>E70/N70</f>
+        <v>1.011303414079525</v>
+      </c>
+    </row>
+    <row r="71" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>95</v>
       </c>
@@ -3953,16 +4994,43 @@
       <c r="J71">
         <v>1657</v>
       </c>
+      <c r="K71">
+        <v>120.328</v>
+      </c>
+      <c r="L71" s="1">
+        <f>D71/K71</f>
+        <v>1.3900255967023467</v>
+      </c>
+      <c r="N71">
+        <v>142.86799999999999</v>
+      </c>
+      <c r="O71" s="1">
+        <f>E71/N71</f>
+        <v>1.0003919702102642</v>
+      </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="I2:I71">
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="6" priority="5" operator="greaterThan">
       <formula>1.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F2:F71">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="5" priority="4" operator="greaterThan">
       <formula>1.05</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L2:L71">
+    <cfRule type="cellIs" dxfId="4" priority="3" operator="greaterThan">
+      <formula>1.05</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O2:O71">
+    <cfRule type="cellIs" dxfId="2" priority="2" operator="greaterThan">
+      <formula>1.03</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="lessThan">
+      <formula>0.97</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>